<commit_message>
exporta dados para serem usados na visualização em d3
</commit_message>
<xml_diff>
--- a/dados/dados-originais/tab_setores.xlsx
+++ b/dados/dados-originais/tab_setores.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A8AE1D-60F8-EF4E-8865-0518B7AA8492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0443B26D-CD96-2249-8E7E-57540EEFE135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tab" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="302">
   <si>
     <t>emp</t>
   </si>
@@ -940,6 +940,9 @@
   </si>
   <si>
     <t>definição</t>
+  </si>
+  <si>
+    <t>Outros setores que não se enquadrem nas definições dos setores destacados.</t>
   </si>
 </sst>
 </file>
@@ -1286,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67D9692-8731-4773-B8DE-FFCD9BB7CE1C}">
   <dimension ref="A1:B264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+    <sheetView topLeftCell="A241" workbookViewId="0">
       <selection activeCell="B253" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -3415,10 +3418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A2:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3561,6 +3564,14 @@
       </c>
       <c r="B17" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
troca nome da coluna na planilha e adapta código
</commit_message>
<xml_diff>
--- a/dados/dados-originais/tab_setores.xlsx
+++ b/dados/dados-originais/tab_setores.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0443B26D-CD96-2249-8E7E-57540EEFE135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFDBCCB-CBE5-FA46-9C4A-F1B22B718948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -939,10 +939,10 @@
     <t>Promoção do turismo regional.</t>
   </si>
   <si>
-    <t>definição</t>
-  </si>
-  <si>
     <t>Outros setores que não se enquadrem nas definições dos setores destacados.</t>
+  </si>
+  <si>
+    <t>def</t>
   </si>
 </sst>
 </file>
@@ -3420,8 +3420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3435,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3571,7 +3571,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrige nome do setor "TRANSPORTES" na tabela original e regera o csv.
</commit_message>
<xml_diff>
--- a/dados/dados-originais/tab_setores.xlsx
+++ b/dados/dados-originais/tab_setores.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFDBCCB-CBE5-FA46-9C4A-F1B22B718948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C55137-0C07-D94F-A37E-AA15DBE8CCE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="301">
   <si>
     <t>emp</t>
   </si>
@@ -928,9 +928,6 @@
   </si>
   <si>
     <t>Tratamento de água e esgoto, drenagem urbana e águas pluviais.</t>
-  </si>
-  <si>
-    <t>TRANSPORTE</t>
   </si>
   <si>
     <t>Serviços de transporte rodoviário, ferroviário e metroviário.</t>
@@ -3420,8 +3417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3435,7 +3432,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3552,10 +3549,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
         <v>297</v>
-      </c>
-      <c r="B16" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3563,7 +3560,7 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3571,7 +3568,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>